<commit_message>
Add gerbers for driver rev 1 and node rev 1.1, updated part tracking and boms for both after jlcpcb and digikey orders. Added new datasheets for driver rev 1
</commit_message>
<xml_diff>
--- a/doc/driver-doc/part_tracking_light_valve_group_driver.xlsx
+++ b/doc/driver-doc/part_tracking_light_valve_group_driver.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianteam/Developer/light-valves/light-valve-group-driver/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianteam/Developer/light-valves/doc/driver-doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D94DB8C-D2CA-B54D-B2C6-54710DC52EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1977C74A-A1F6-2E48-A38D-E283B1124B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15600" yWindow="500" windowWidth="36000" windowHeight="21300" xr2:uid="{C42DAD60-93F4-1A4B-8199-2F910E4FACBD}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21120" xr2:uid="{C42DAD60-93F4-1A4B-8199-2F910E4FACBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="77">
   <si>
     <t>Part</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Alternate(s)</t>
   </si>
   <si>
-    <t>MCP15A0305</t>
-  </si>
-  <si>
     <t>Inverting/non-inverting line driver</t>
   </si>
   <si>
@@ -61,21 +58,9 @@
     <t>MIC4425/8</t>
   </si>
   <si>
-    <t>AP1507-D5-13</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/diodes-incorporated/AP1507-D5-13/5768439</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/filter/pmic-voltage-regulators-dc-dc-switching-regulators/739?s=N4IgjCBcpgbFoDGUBmBDANgZwKYBoQB7KAbRACZYB2S%2BAym6ke6gZiquYuoBYAGAKxcGPMJxZVRADmG84sqrD7juisKwWxYATk1VdE-eQVS%2BxiaYj1tPVuSsUbpjQQF8p1PsKfvvPKdoGjv7aMtY82uRBURHkYcHadn6JDlFurKnabrDmjtmZboreAmB8dHmlQtYlYFV5UfFpUblpGQUZuTxU6XWtAjzFrJHF-OVp-CrjgsVuA9UlXvNgcyCsgjyw8WsCAh5c27Cl%2B4KH5VQZiVw8EQG5knF1bjZiXAsC5CqS7A6S1-G-XS4vykdz%2BLhAkmoQUhpiutioewIkkkPy6ES4zgE4Kk3TcGMUUgcOJ0QRxVD4KxxUkRICpOPxAWxCOGBBxNnK1L4tSuUWoKm0Oh2VyoYkBBG0NG5rmW5GuXAldnBCtY5QVUiV50J8shGo2KwlGyCBps2oiKg2%2BnkBFKUi6KhtXSCDth1vcuxWNsOKx4AgRWtdHiiXE9WOD7lgAnKnoRYY8LpAGzEAid4YFscFsZoi3A7hBdRtto9udY8QLNIL2gcNpsKYCeOtYHI7uDjd2%2BcbOXBGz47m9klCTtssBLwaHQ1H7GUE8Y09E09206UE4C2eWQzAVdslcHQyF1q3vtH-A3R7MUY2blXESG4NqYBx2a6UQywZ2Znzb8or6eUZ2HW-GS3n%2BSTWn%2B-QAXu4DJrKQGJJGwYRuc%2BaISqCG%2BuO1oRuq9oRikwbUuS9rUmywbbiy4CRGYToGnO1o0Ss5A9oxvRMaw4KMWuLS1LKYy1EMkw%2BuoYxKDs5SbO4XL7HW4EEPwZhrFc6yyop-SsHU-CqQ4GnXI%2B6wjrJ6wRip-SdOoojlKIrCiOaZk0pZESPmZWQgAAugQAAOAAuUAgAAyp5ABOACWAB2ADmIAAL4EDoCAgMgkDoNg%2BBEKQCZ8IklwGTYCluSAXk%2Bf5wXhVFrKcNA8WoJguAEMQkBkPw5D6asApGXlBWQH5gWhRF0XgEcFUJUlNWpfV6Xqr4BnqkuU0lkE-DqtoumLVp7g3q5HneZ1RU9aV4BBoNVXJbVaVvrRIBvgErxfPEvq2OCsCNTkryROwL1NQ9GUvJhai5HA3QmtaTbKB6DDfft1DLMGDRMNaGSqcG8MvnDPqhMIXI5C0XLJh6IrUlGNCMsG5ytcTETPdaigg8TjCNB8jFjB8YDkQzggsW27HuDB6Mgs1socGxwh2mUwh2A%2Bsg5PSLA5IcwimOSjSJDQKxrCE0KyudcZfuKWiy66TYnq6ij%2BKOjHota6rXht%2BVbV1xW9a45xxUN1UpXVZBrs4o4Rla4ARLYHpPmpr73mjoElOqr6RGK4BeuDcC7BT4C2smpbEczpGCEcdEcfmThynR5zkujZiNsIfHTPQ95lJM5AfakTU%2BpMJaakLu5jIalbCL6j0tD3mzCH6JRy4ob3tbbO0lX1AC0xiHZAgUAK5u6d8quZFfXwBVQUACY%2BdPpQOB1IBcJ5ACe7k4D5aBYMgBAAI7nz5UWRUAA</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>12V adjustable switching regulator</t>
-  </si>
-  <si>
     <t>3V3 fixed switching regulator</t>
   </si>
   <si>
@@ -86,14 +71,217 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/filter/pmic-voltage-regulators-dc-dc-switching-regulators/739?s=N4IgjCBcpgbFoDGUBmBDANgZwKYBoQB7KAbRACZYB2S%2BAym6ke6gZiquYuoBYAGAKxcGPMJxZVRADmG84sqrD7juisKwWxYATk1VdE-eQVS%2BxiaYj1tPVuSsUbpjQQF8p1PsKfvvPKdoGjv7aMtY82uRBURHkYcHadn6JDlFurKnabrDmjtmZboreAmB8dHmlQtYlYFV5UfFpUblpGQUZuTxU6XWtAjzFrJHF-OVp-CrjgsVuA9UlXvNgcyCsgjyw8WsCAh5c27Cl%2B4KH5VQZiVw8EQG5knF1bjZiXAsC5CqS7A6S1-G-XS4vykdz%2BLhAkmoQUhpiutioewIkkkPy6ES4zgE4Kk3TcGMUUgcOJ0QRxVD4KxxUkRICpOPxAWxCOGBBxNnK1L4tSuUWoKm0Oh2VyoYkBBG0NG5rmW5GuXAldnBCtY5QVUiV50J8shGo2KwlGyCBps2oiKg2%2BnkBFKUi6KhtXSCDth1vcuxWNsOKx4AgRWtdHiiXE9WOD7lgAnKnoRYY8LpAGzEAid4YFscFsZoi3A7hBdRtto9udY8QLNIL2gcNpsKYCeOtYHI7uDjd2%2BcbOXBGz47m9klCTtssBLwaHQ1H7GUE8Y09E09206UE4C2eWQzAVdslcHQyF1q3vtH-A3R7MUY2blXESG4NqYBx2a6UQywZ2Znzb8or6eUZ2HW-GS3n%2BSTWn%2B-QAXu4DJrKQGJJGwYRuc%2BaISqCG%2BuO1oRuq9oRikwbUuS9rUmywbbiy4CRGYToGnO1o0Ss5A9oxvRMaw4KMWuLS1LKYy1EMkw%2BuoYxKDs5SbO4XL7HW4EEPwZhrFc6yyop-SsHU-CqQ4GnXI%2B6wjrJ6wRip-SdOoojlKIrCiOaZk0pZESPmZWQgAAugQAAOAAuUAgAAyp5ABOACWAB2ADmIAAL6yRA0AgMgkDoNg%2BBEKQqylOw4JWV8DhDFyPquR53mQH5gWhRF0UgDoCDxagmC4AQxCQGQ-CJJcBk2ApbkgF5Pn%2BcF4VRaynBxQlSUNalzUJvJWwCkZ3W9SV-XlUN4BHKNdXJY1aX8OqvgGeqS4HSWQS7XlinqpWF03oVPXFaVA0Va45w1WN9UpU1ZBrs4o4Rla4ARLYHpPmpr73qE373rBso4csLyYbsOT4T6EPWsRYDUYIRx0Rx%2BZOHKdHnOSwhMY2wh8dM9D3mUkzkOQbGpPTPqTCWmrCAeYyGld9C%2BrAPAtLzmzCH6JTCMS7C3YtD0rZVYj6K9m0TZ94AotyC33ctg2VQAtMYG2QIFACuH1pXUuguZFlXwHFQUACY%2BdrpQOFLXCeQAnu5OA%2BWgWDIAQACO7s%2BVFkVAA</t>
+  </si>
+  <si>
+    <t>SP485CN-L/TR</t>
+  </si>
+  <si>
+    <t>RS485 transviever</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/maxlinear-inc/SP485CN-L-TR/2471959</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/filter/interface-drivers-receivers-transceivers/710?s=N4IgjCBcoKwOwA4qgMZQGYEMA2BnApgDQgD2UA2iAMwCcNADACxwjG0MxIC6xADgC5QQAZX4AnAJYA7AOYgAvsQC0AJmQg0kcQFcipCiBisQNEF3mKQANnUSAJkKVh6EPoMghj-AJ698QzFw0CyA</t>
+  </si>
+  <si>
+    <t>RT8258GJ6</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/richtek-usa-inc/RT8258GJ6/2546043</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/filter/pmic-voltage-regulators-dc-dc-switching-regulators/739?s=N4IgjCBcpgbFoDGUBmBDANgZwKYBoQB7KAbRACZYB2S%2BAym6ke6gZiquYuoBYAGAKxcGPMJxZVRADmG84sqrD7juisKwWxYATk1VdE-eQVS%2BxiaYj1tPVuSsUbpjQQF8p1PsKfvvPKdoGjv7aMtY82uRBURHkYcHadn6JDlFurKnabrDmjtmZboreAmB8dHmlQtYlYFV5UfFpUblpGQUZuTxU6XWtAjzFrJHF-OVp-CrjgsVuA9UlXvNgcyCsgjyw8WsCAh5c27Cl%2B4KH5VQZiVw8EQG5knF1bjZiXAsC5CqS7A6S1-G-XS4vykdz%2BLhAkmoQUhpiutioewIkkkPy6ES4zgE4Kk3TcGMUUgcOJ0QRxVD4KxxUkRICpOPxAWxCOGBBxNnK1L4tSuUWoKm0Oh2VyoYkBBG0NG5rmW5GuXAldnBCtY5QVUiV50J8shGo2KwlGyCBps2oiKg2%2BnkBFKUi6KhtXSCDth1vcuxWNsOKx4AgRWtdHiiXE9WOD7lgAnKnoRYY8LpAGzEAid4YFscFsZoi3A7hBdRtto9udY8QLNIL2gcNpsKYCeOtYHI7uDjd2%2BcbOXBGz47m9klCTtssBLwaHQ1H7GUE8Y09E09206UE4C2eWQzAVdslcHQyF1q3vtH-A3R7MUY2blXESG4NqYBx2a6UQywZ2Znzb8or6eUZ2HW-GS3n%2BSTWn%2B-QAXu4DJrKQGJJGwYRuc%2BaISqCG%2BuO1oRuq9oRikwbUuS9rUmywbbiy4CRGYToGnO1o0Ss5A9oxvRMaw4KMWuLS1LKYy1EMkw%2BuoYxKDs5SbO4XL7HW4EEPwZhrFc6yyop-SsHU-CqQ4GnXI%2B6wjrJ6wRip-SdOoojlKIrCiOaZk0pZESPmZWQgAAugQAAOAAuUAgAAyp5ABOACWAB2ADmIAAL4EDoCAgMgkDoNg%2BBEKQCZ8IklwGTYCluSAXk%2Bf5wXhVFrKcNA8WoJguAEMQkBkPw5D6asApGXlBWQH5gWhRF0XgEcFUJUlNWpfV6Xqr4BnqkuU0lkE-DqtoumLVp7g3q5HneZ1RU9aVIDoXFQ3VSldVkGuzijhGVrgBEtgek%2BamvveoTfvesGyjhywvJhuw5PhPovdaxFgNRghHHRHH5k4cp0ec5LCExjbCHx0z0PeZSTOQTUvvQTU%2BpMJaasIB5jIalbCL6sA8C0lObMIfolMIxLsBt%2BVbV1xW9QQAC0xiDVAgUAK4nWldS6C5kV9fAFVBQAJj53OlA4HUgFwnkAJ7uTgPloFgyAEAAjhrPlRZFQA</t>
+  </si>
+  <si>
+    <t>1-15V adjustable switching regulator for 12v-&gt;5V</t>
+  </si>
+  <si>
+    <t>MCP14A0305</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/filter/common-mode-chokes/839?s=N4IgjCBcoGwJxVAYygMwIYBsDOBTANCAPZQDaIALAAxwDMdIAuoQA4AuUIAymwE4CWAOwDmIAL6EwcAByIQKSBhwFiZcACYwtdTBCF6MGAFYmrDpG58hoiRobR5aLHkIlI5MFWkB2Cur3gYMY0AWAUtNJUtKFGRmDS0ZLSFEYyodIZUqFw3rTeVAGaRrRUJoTqEbmy5UbeMH6FMPTq1SAtdXmFcGG0uoTwMOoIhMktwyDSRsneAXAU3lOhVFQw3hCStUPr4PWxiTsUMtvx6t6n2WA6BZJ0mn1tYHWehUVU-uV5tPOFRjBBZW1crQSoVvJNvuVpMZDF0aMkAjAEvDJNQwhRTCB2JweAIROIbhU5AolC5VO42r0Fq0KqsvoVUdJtupYpN9joadT6nN0eUznA4qDfEFClD1ITITI5l1urEAiUxdRQlIFtdKLFUgEUkYxZqEt4ZoRtYztrEqBQTb5gQFUhV9jAaI9QqtUjyNKswqEdGF3hppgDLjJVqFaGBiscvqlWlo-HTJL1lq6tGdEYUqKGpZI1hlE2dpAxMzpDqE6lRfMXk-6wToAWK1nAfepSxQi%2BU4bLyvN8vcKi0gx8vn2KaiG4YvSLS14unl1K6Ws2dHKzXnxmdm9tjFMAfWk0tmWBjqHs0q5lpQn4zQhmJjzJZcTZCABafwOBR8ACuKjc5C3TDEthMDgsFAYCsEBkDMrYugOPwAAmnAPp42xYhYARsAAniwuCcOg2AoH%2BQA</t>
+  </si>
+  <si>
+    <t>much cheaper alternatives in qty 10 vs. qty. 1</t>
+  </si>
+  <si>
+    <t>SRF4532-1R0Y</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/bourns-inc/SRF4532-1R0Y/6134003</t>
+  </si>
+  <si>
+    <t>Driver data differential common mode choke</t>
+  </si>
+  <si>
+    <t>4-line screw block terminal</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/würth-elektronik/691137710004/6644053</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/filter/terminal-blocks-wire-to-board/371?s=N4IgjCBcpgDA7AViqAxlAZgQwDYGcBTAGhAHsoBtEAJlgGYwA2eEAXRIAcAXKEAZS4AnAJYA7AOYgAviTAAWABwtoIdJGz5iZSiDmxYcgJywQJPQcN1Tu-UbnXzR5GduGWLgwoVtOPSPyExSRlwQwVDFFVMXEISckgqE1YQ6iZvFTUNWO0E8B8Qbl4ASVEuAnECQWkSAFpqSLUhAFcteKpnEAjkkMZI4QATXhq4CF9eay4ATw4CXiw8dCkpIA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/würth-elektronik/150080GS75000/4489915</t>
+  </si>
+  <si>
+    <t>0805 green LED</t>
+  </si>
+  <si>
+    <t>150080GS75000</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/filter/led-indication-discrete/105?s=N4IgjCBcoCwGxVAYygMwIYBsDOBTANCAPZQDa4ATBQBzUQC6hADgC5QgDKLATgJYB2AcxABfQnACciECkgYcBYmRAwADBIDMmkIxCt2XPkNGEwE6lOgy0WPIRKRyqnWJABaCtNk8AroofkAKwghFL0Iq7BVkxQYMwxkBSBrghWvAAm7G5gqhDMbJAgISAsAJ5MuOzo2CgRQA</t>
+  </si>
+  <si>
+    <t>0805s (alternate link) about 10c more than 0605s</t>
+  </si>
+  <si>
+    <t>150080SS75000</t>
+  </si>
+  <si>
+    <t>0805 red LED</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/würth-elektronik/150080SS75000/4489921</t>
+  </si>
+  <si>
+    <t>^</t>
+  </si>
+  <si>
+    <t>Buck regulator schottky</t>
+  </si>
+  <si>
+    <t>SK53AFL-TP</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/micro-commercial-co/SK53AFL-TP/4966275</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/filter/diodes-rectifiers-single/280?s=N4IgjCBcoGwJxVAYygMwIYBsDOBTANCAPZQDaIALAAxwDMdIAuoQA4AuUIAymwE4CWAOwDmIAL6E4YCohApIGHAWJlwMAOwBWODMIAmKmG27w6mFXUm9e9WDh6Q%2BiuvVUYjkHrrq9JnxQoIQgAOGGC9d0IwKj1NMCDwCgMKBH1pehlmEHZOHgERcSi4YIRoOTQsPEISSHIqJglPCwgy%2BUUqlVqQWioAAgA1JlYOSBAAVUF%2BNgB5VABZXHRsAFdeXEKQAFoHVqg%2BZeUa8k0PBEYxRpOyligwVhvIWMb3Mv4AE05N6ISc0Y82ACeLHWoyWKAuQA</t>
+  </si>
+  <si>
+    <t>NRS8040T150MJGJ</t>
+  </si>
+  <si>
+    <t>Buck regulator inductor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/taiyo-yuden/NRS8040T150MJGJ/2666011</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/filter/fixed-inductors/71?s=N4IgjCBcoGwJxVAYygMwIYBsDOBTANCAPZQDaIALAAxwDMdIAuoQA4AuUIAymwE4CWAOwDmIAL6EwAJjAJoIFJAw4CxMuBgB2AKxwKISVNoUp%2Bw9qqaqB8KbAwAHDelawZ27qkJDDijudSDvZOhnAOWgFwmtHOtGDacbHGVCHgtHGysRS6qWDGRu55MFRUhbS6ebGaUo6x8LRSNlJU8XrOmmAOvu2BDJLVMBTe4Jr0g%2B1DMBD9fon9xZqFOr6N-QPa7Q41G-1wVNo7I3sUMM4OJVKaTZeyqyDNFENXhM0JFKnNxQdNVI6lP4shj8trQPil9tN7jRLtYXik4NpTi8wC0wJCZL8tk0-FYkfdaOCPnFaDEXnEpBSmnE9ocjPYTFS6XijIEImTjGyQI4LO8qRz0clpHydMMChQwM97jAYDV0dpTKT7vK4DKmvLfO4pNpqPE1Y8tXrFrD7ucrB9HF1jTU4JdzXAJZLrdoUU0rNQPh0GrTqvtaE06NVNVsvH6XiDOYEGhRQybQfQbAT3nBRQjkx8VXFmSqDpqotLaXmjP6gtUbIHxTZpW48ZowpyRdqyzASXdwls8VtSoctmF3Da8pKVVWbHR0n36PYR9Qas4qFq0SOHKDCpZBrlpPZISiotpJWjtF1CicZFvHg1T0MSc4k83r4tb5JnQk99roy-Aor4kuH%2BBEb9hpuNAAc28R3PYJLZGcxh9OAXTBM49qaD%2BRh7C0TRfJ0TCsBwkDcHwQiiBI4BhHIyBoFgeCECQkDkNYjBEc0DhXPIijKJRag0b%2BAAEACtAASWEgOwnAAKqCPwbAAPKoAAsrg6DYAArrwuDiHCXSIAo5EqFR6hSAAdFIXEAIJNIZ2gmWZtCWS8%2BnlDZ9z6RQDkGX4Ln6RZpm2TA7maL5nlmQ47lwA51leSAtD6TQoX6WAMX2DFRnhZFYUJk5MUBYQkU%2Bcl%2BkwJlEX6X5uU6DFQW5b4MUheFzk1bFDkULF5U2I1SUtYZxXtZcnWEI1qW9eldXZA1HkjTl7U9ZQ%2BnNQNS4jdVNgFdoUWBA5y1UP1IDLXF4XLW1hB7ftW12Wtg2LU5S2jbteWnZNy0zVyDkwOZT0neFz21ZWV1fZNz0PZNmjfYQgPjcDRUOQ9DiGRDQMgFDoNw%2BD4ULYQcDQ8jSMjtNDkojjVD1eFKKY5IYDE%2BApMPdIOMGQVbg4wjnQuUdRiw1qrOAwVq3JVQoWbbQ43MEJOEgGJEnSXJCnKapREALSNCxUB8IpqjUeQhwIPRRGnPI-AACacDLKKQsJuE2GwACeLCqbhCkoGIYhAA</t>
+  </si>
+  <si>
+    <t>Buck regulator input cap(s)</t>
+  </si>
+  <si>
+    <t>CL31B106KBHNNNE</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL31B106KBHNNNE/5961251</t>
+  </si>
+  <si>
+    <t>CL21A226MAYNNNE</t>
+  </si>
+  <si>
+    <t>Buck regulator output cap(s)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL21A226MAYNNNE/10479857</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/filter/ceramic-capacitors/60?s=N4IgjCBcpgLFoDGUBmBDANgZwKYBoQB7KAbRACYBmADgHYaQBdAgBwBcoQBlNgJwEsAdgHMQAXwJgAnNSkIQySOmz4ipEAAYmEihthzoC1JlwFikMuXIACAK0AxJqw6QQAVUH82AeRQBZHDQsAFdeHHECAFpyeUU%2BYNVzMgBWEAI5RjEdVMMWKDBWPMhyZJ0ANnl%2BABNOSLANCGdONJA2AE8WcNcg5CygA</t>
+  </si>
+  <si>
+    <t>CL21B103KBANNNC</t>
+  </si>
+  <si>
+    <t>Buck regulator BOOT cap</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL21B103KBANNNC/3886673</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/filter/ceramic-capacitors/60?s=N4IgjCBcpgLFoDGUBmBDANgZwKYBoQB7KAbRACYBmADgHYaQBdAgBwBcoQBlNgJwEsAdgHMQAXwJgAbAhDJI6bPiKkQlAJyVy6kAWqVaYCHtiwpABl3g4scuStHYtajMmxqRy8xDtOPASLikurUOtByqJi4BMSQZF4SFOawYaC%2BkCAAqoL8bADyKACyOGhYAK68OFZlnIIAYlYAtkKcYJYEjWgAHq2WiQC09uHyfGXKsWQArFY6jGKJ0%2BEsUOSsy5Dkk4ky4fwAJpz9bcY%2BHBlWbACeLFUZpcgEAI5XnOJiQA</t>
+  </si>
+  <si>
+    <t>RC0805FR-0791KL</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/filter/chip-resistor-surface-mount/52?s=N4IgjCBcpgbFoDGUBmBDANgZwKYBoQB7KAbRAGYBOAJgBZ4CrzrKRHKAGAVnLZAA5yAdjAQC-WvQ58wtDpS4NwXIXN4E6YYfAC6BAA4AXKCADKhgE4BLAHYBzEAF8NHflwQgjJgKo2rhgHkUAFkcNCwAVwscPgiTAGsAgAsAWyw%2BFNsTSjEQFLQAD2yIZxAAWmoPZEhLCPwiUhB3AlYdR1L4aBArABMTMrAOXK9IED5DAE99GNHw5HagA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/RC0805FR-0791KL/728202</t>
+  </si>
+  <si>
+    <t>Buck regulator 91k divider resistor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/filter/chip-resistor-surface-mount/52?s=N4IgjCBcpgbFoDGUBmBDANgZwKYBoQB7KAbXAFYB2AFgAYBmEA%2BgTnoCYWmQAOeysBAI9q1WLRABdAgAcALlBABlOQCcAlgDsA5iAC%2BBdrR7kEIZJHTZ8RUuEoA6dgAIA1gHkAFgFss3MI7Ubl6%2B-rAOLME%2BftIg8ooAqprqcu4oALI4aFgArqo4%2BgQAtOxmFmo5NsSQZKYEXJJ6BiDw0CDqACaKRWC0QnEKkCDccgCeMgVD2chNQA</t>
+  </si>
+  <si>
+    <t>RMCF0805FT17K4</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0805FT17K4/1712744</t>
+  </si>
+  <si>
+    <t>Buck regulator 17.4k divider resistor</t>
+  </si>
+  <si>
+    <t>ECQ-E2475KF</t>
+  </si>
+  <si>
+    <t>FET driver 4.7uF film bypass cap</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/panasonic-electronic-components/ECQ-E2475KF/56516</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/filter/film-capacitors/62?s=N4IgjCBcpgnAHLKoDGUBmBDANgZwKYA0IA9lANogAMIAugL7EBMVALEtCGpFnkaRRCsAdAHYABAFaAYnWIAHAC5QQAVQB2AS0UB5dAFl8mXAFcATvhCMQAWibIuURWZP8ykSkmIBWOvWsAbA6aACYqNmBUEArKkCAgxIoAnvKWccZoxACOySpW9EA</t>
+  </si>
+  <si>
+    <t>FET driver 0.1uF ceramic bypass cap</t>
+  </si>
+  <si>
+    <t>MMBZ9V1ALT1G</t>
+  </si>
+  <si>
+    <t>RS485 data TVS</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/onsemi/MMBZ9V1ALT1G/921147</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/filter/tvs-diodes/144?s=N4IgjCBcpg7ATATiqAxlAZgQwDYGcBTAGhAHsoBtEeEAXRIAcAXKEASQDsmCBzAgJxABfEnADMNaCHSRs%2BYmUohEsACwAGMSBKJ4AVgnbl%2BpEYAcZgGyqz5i%2Bst3EYWyTPOz6889ixvY9T83RADHYNV4GmC9CKMVDUd6EGZWAGUmfgBLDh5hUUR3FGlMXEISckgqL1oREABaSTQoDIBXBQqqPTi6IVquqQYoMEZByH1axylMgBNWOrB1CEYWSBAjJgBPBgJWLDx0XqA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/koa-speer-electronics-inc/RCWCTE/11476558?s=N4IgTCBcDaIEoGEDqCAqBREBdAvkA</t>
+  </si>
+  <si>
+    <t>RCWCTE</t>
+  </si>
+  <si>
+    <t>Square grounding bar test point</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -121,8 +309,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,17 +627,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21AADDCC-C8AC-434D-96DB-539CB8F7965B}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.83203125" customWidth="1"/>
     <col min="4" max="6" width="43.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -467,98 +657,321 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>691137710004</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" t="s">
+        <v>52</v>
+      </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>